<commit_message>
verigen : add default clock, add vfunctions ($LOG2, $RANGE, $DEMUX_BY_EN, $MULTICYCLE)
</commit_message>
<xml_diff>
--- a/Common/doc/verigen/media/instruction_clock.xlsx
+++ b/Common/doc/verigen/media/instruction_clock.xlsx
@@ -8,17 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Profiles\Common\doc\verigen\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFA5F51B-1ECF-4EEC-B710-53BE948FCAF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5021EC6B-096F-4436-881C-B94A3C19A48B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2970" yWindow="270" windowWidth="18390" windowHeight="15300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="6" r:id="rId1"/>
     <sheet name="new" sheetId="1" r:id="rId2"/>
     <sheet name="set_reset" sheetId="2" r:id="rId3"/>
-    <sheet name="set_speed" sheetId="3" r:id="rId4"/>
-    <sheet name="find" sheetId="4" r:id="rId5"/>
-    <sheet name="is_valid" sheetId="5" r:id="rId6"/>
+    <sheet name="get_reset" sheetId="7" r:id="rId4"/>
+    <sheet name="set_speed" sheetId="3" r:id="rId5"/>
+    <sheet name="set_default" sheetId="8" r:id="rId6"/>
+    <sheet name="find" sheetId="4" r:id="rId7"/>
+    <sheet name="is_valid" sheetId="5" r:id="rId8"/>
+    <sheet name="get_default" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="57">
   <si>
     <t>clock</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -223,6 +226,56 @@
   </si>
   <si>
     <t>확인할 clock 객체.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>:get_reset</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>clock에 할당된 reset 을 반환</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>function clock:get_reset()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>clock에 할당된 reset을 반환한다.
+할당된 reset 이 없다면, 기본 reset 신호가 반환된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>.get_default</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기본 클럭을 얻는다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>:set_default</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>현 클럭을 기본 클럭으로 설정한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>function clock:set_default()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>현재 클럭을 기본 클럭으로 설정한다.
+처음 생성하는 클럭을 기본 클럭으로 설정하며, 별도로 특정 클럭을 명시적으로 클럭으로 설정할 때 사용한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>function clock.get_default()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기본 클럭을 반환한다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -558,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63D1552F-D2B8-4AD9-9ECE-3CAF9162E459}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -616,35 +669,68 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -727,7 +813,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -784,8 +870,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F3A3807-3398-4A4F-B1BD-9BC569F34502}">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB27B6E5-00A6-4606-85A2-F16E7242B9CD}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -810,6 +896,58 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F3A3807-3398-4A4F-B1BD-9BC569F34502}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="55.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -844,7 +982,60 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F725EA3-D526-4AE1-8C1D-CD70760546C0}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="55.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77748D98-643E-48A6-98CF-87576597A7B3}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -905,11 +1096,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B1EF6B3-56F8-4472-8BF2-44B9BE839153}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -963,4 +1154,56 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF5A31A6-3A10-49D1-8C10-696596C7A595}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="55.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>